<commit_message>
Updated charts. Up Next: Add an entire workbook that can be read from and perform EDA upon it.
</commit_message>
<xml_diff>
--- a/Data/Input Data - Optix.xlsx
+++ b/Data/Input Data - Optix.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/piyushkumar/Documents/GitHub/sales-revenue-tool/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1A04273-4D20-0543-A8BD-06D6534697E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91A14F14-B49A-E046-B0AC-7E16063D4D86}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4520" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{901DEC1D-347C-854D-A679-0D04B39C13DF}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" xr2:uid="{901DEC1D-347C-854D-A679-0D04B39C13DF}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,9 +37,6 @@
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>Month</t>
-  </si>
   <si>
     <t>salesUnits</t>
   </si>
@@ -90,6 +87,9 @@
   </si>
   <si>
     <t>tupSchemeDA</t>
+  </si>
+  <si>
+    <t>date</t>
   </si>
 </sst>
 </file>
@@ -210,9 +210,6 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="16" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -220,9 +217,6 @@
       <alignment horizontal="right" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="16" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
@@ -233,6 +227,12 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="17" fontId="3" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -569,70 +569,73 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF954B16-2EA8-8445-A958-34EBBF944F43}">
   <dimension ref="A1:U38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S2:U38"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="30" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="10" t="s">
+      <c r="D1" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="E1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="10" t="s">
+      <c r="G1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="10" t="s">
+      <c r="H1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="10" t="s">
+      <c r="I1" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="K1" s="10" t="s">
+      <c r="L1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="10" t="s">
+      <c r="M1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A2" s="3">
+      <c r="A2" s="12">
         <v>45433</v>
       </c>
       <c r="B2" s="1">
@@ -644,10 +647,10 @@
       <c r="D2" s="1">
         <v>1</v>
       </c>
-      <c r="E2" s="4">
+      <c r="E2" s="3">
         <v>66</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>24</v>
       </c>
       <c r="G2" s="1">
@@ -656,10 +659,10 @@
       <c r="H2" s="1">
         <v>233</v>
       </c>
-      <c r="I2" s="13">
+      <c r="I2" s="11">
         <v>1.4</v>
       </c>
-      <c r="J2" s="13">
+      <c r="J2" s="11">
         <v>1.5</v>
       </c>
       <c r="K2" s="1">
@@ -668,25 +671,25 @@
       <c r="L2" s="1">
         <v>235</v>
       </c>
-      <c r="M2" s="6">
-        <v>0</v>
-      </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
-      <c r="O2" s="6">
+      <c r="M2" s="5">
+        <v>0</v>
+      </c>
+      <c r="N2" s="5">
+        <v>0</v>
+      </c>
+      <c r="O2" s="5">
         <v>104</v>
       </c>
-      <c r="P2" s="11"/>
-      <c r="Q2" s="11"/>
-      <c r="R2" s="11">
+      <c r="P2" s="9"/>
+      <c r="Q2" s="9"/>
+      <c r="R2" s="9">
         <v>66.356999999999999</v>
       </c>
-      <c r="S2" s="13"/>
-      <c r="T2" s="13"/>
+      <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A3" s="3">
+      <c r="A3" s="12">
         <v>45464</v>
       </c>
       <c r="B3" s="1">
@@ -698,10 +701,10 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="E3" s="4">
+      <c r="E3" s="3">
         <v>68</v>
       </c>
-      <c r="F3" s="5">
+      <c r="F3" s="4">
         <v>31</v>
       </c>
       <c r="G3" s="1">
@@ -710,10 +713,10 @@
       <c r="H3" s="1">
         <v>273</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="11">
         <v>1.4</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="11">
         <v>1.5</v>
       </c>
       <c r="K3" s="1">
@@ -722,26 +725,26 @@
       <c r="L3" s="1">
         <v>270</v>
       </c>
-      <c r="M3" s="6">
-        <v>0</v>
-      </c>
-      <c r="N3" s="6">
-        <v>0</v>
-      </c>
-      <c r="O3" s="6">
+      <c r="M3" s="5">
+        <v>0</v>
+      </c>
+      <c r="N3" s="5">
+        <v>0</v>
+      </c>
+      <c r="O3" s="5">
         <v>100</v>
       </c>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11">
+      <c r="P3" s="9"/>
+      <c r="Q3" s="9"/>
+      <c r="R3" s="9">
         <v>68.370999999999995</v>
       </c>
-      <c r="S3" s="13"/>
-      <c r="T3" s="13"/>
-      <c r="U3" s="12"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="10"/>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A4" s="3">
+      <c r="A4" s="12">
         <v>45494</v>
       </c>
       <c r="B4" s="1">
@@ -753,10 +756,10 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="E4" s="4">
+      <c r="E4" s="3">
         <v>68</v>
       </c>
-      <c r="F4" s="5">
+      <c r="F4" s="4">
         <v>29</v>
       </c>
       <c r="G4" s="1">
@@ -765,10 +768,10 @@
       <c r="H4" s="1">
         <v>265</v>
       </c>
-      <c r="I4" s="13">
+      <c r="I4" s="11">
         <v>1.4</v>
       </c>
-      <c r="J4" s="13">
+      <c r="J4" s="11">
         <v>1.5</v>
       </c>
       <c r="K4" s="1">
@@ -777,25 +780,25 @@
       <c r="L4" s="1">
         <v>227</v>
       </c>
-      <c r="M4" s="6">
-        <v>0</v>
-      </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
-      <c r="O4" s="6">
+      <c r="M4" s="5">
+        <v>0</v>
+      </c>
+      <c r="N4" s="5">
+        <v>0</v>
+      </c>
+      <c r="O4" s="5">
         <v>100</v>
       </c>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11">
+      <c r="P4" s="9"/>
+      <c r="Q4" s="9"/>
+      <c r="R4" s="9">
         <v>67.995000000000005</v>
       </c>
-      <c r="S4" s="13"/>
-      <c r="T4" s="13"/>
+      <c r="S4" s="11"/>
+      <c r="T4" s="11"/>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A5" s="3">
+      <c r="A5" s="12">
         <v>45525</v>
       </c>
       <c r="B5" s="1">
@@ -807,10 +810,10 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="E5" s="4">
+      <c r="E5" s="3">
         <v>68</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="4">
         <v>28</v>
       </c>
       <c r="G5" s="1">
@@ -819,10 +822,10 @@
       <c r="H5" s="1">
         <v>267</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="11">
         <v>1.4</v>
       </c>
-      <c r="J5" s="13">
+      <c r="J5" s="11">
         <v>1.5</v>
       </c>
       <c r="K5" s="1">
@@ -831,25 +834,25 @@
       <c r="L5" s="1">
         <v>205</v>
       </c>
-      <c r="M5" s="6">
-        <v>0</v>
-      </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
-      <c r="O5" s="6">
+      <c r="M5" s="5">
+        <v>0</v>
+      </c>
+      <c r="N5" s="5">
+        <v>0</v>
+      </c>
+      <c r="O5" s="5">
         <v>99</v>
       </c>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11">
+      <c r="P5" s="9"/>
+      <c r="Q5" s="9"/>
+      <c r="R5" s="9">
         <v>68.004999999999995</v>
       </c>
-      <c r="S5" s="13"/>
-      <c r="T5" s="13"/>
+      <c r="S5" s="11"/>
+      <c r="T5" s="11"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
+      <c r="A6" s="12">
         <v>45556</v>
       </c>
       <c r="B6" s="1">
@@ -861,10 +864,10 @@
       <c r="D6" s="1">
         <v>1</v>
       </c>
-      <c r="E6" s="4">
+      <c r="E6" s="3">
         <v>69</v>
       </c>
-      <c r="F6" s="5">
+      <c r="F6" s="4">
         <v>27</v>
       </c>
       <c r="G6" s="1">
@@ -873,10 +876,10 @@
       <c r="H6" s="1">
         <v>265</v>
       </c>
-      <c r="I6" s="13">
+      <c r="I6" s="11">
         <v>1.4</v>
       </c>
-      <c r="J6" s="13">
+      <c r="J6" s="11">
         <v>1.5</v>
       </c>
       <c r="K6" s="1">
@@ -885,25 +888,25 @@
       <c r="L6" s="1">
         <v>192</v>
       </c>
-      <c r="M6" s="6">
-        <v>0</v>
-      </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
-      <c r="O6" s="6">
+      <c r="M6" s="5">
+        <v>0</v>
+      </c>
+      <c r="N6" s="5">
+        <v>0</v>
+      </c>
+      <c r="O6" s="5">
         <v>94</v>
       </c>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11">
+      <c r="P6" s="9"/>
+      <c r="Q6" s="9"/>
+      <c r="R6" s="9">
         <v>69.366</v>
       </c>
-      <c r="S6" s="13"/>
-      <c r="T6" s="13"/>
+      <c r="S6" s="11"/>
+      <c r="T6" s="11"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A7" s="3">
+      <c r="A7" s="12">
         <v>45586</v>
       </c>
       <c r="B7" s="1">
@@ -915,10 +918,10 @@
       <c r="D7" s="1">
         <v>1</v>
       </c>
-      <c r="E7" s="4">
+      <c r="E7" s="3">
         <v>68</v>
       </c>
-      <c r="F7" s="5">
+      <c r="F7" s="4">
         <v>26</v>
       </c>
       <c r="G7" s="1">
@@ -927,10 +930,10 @@
       <c r="H7" s="1">
         <v>254</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <v>1.4</v>
       </c>
-      <c r="J7" s="13">
+      <c r="J7" s="11">
         <v>1.5</v>
       </c>
       <c r="K7" s="1">
@@ -939,25 +942,25 @@
       <c r="L7" s="1">
         <v>211</v>
       </c>
-      <c r="M7" s="6">
-        <v>0</v>
-      </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
-      <c r="O7" s="6">
+      <c r="M7" s="5">
+        <v>0</v>
+      </c>
+      <c r="N7" s="5">
+        <v>0</v>
+      </c>
+      <c r="O7" s="5">
         <v>99</v>
       </c>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11">
+      <c r="P7" s="9"/>
+      <c r="Q7" s="9"/>
+      <c r="R7" s="9">
         <v>68.033000000000001</v>
       </c>
-      <c r="S7" s="13"/>
-      <c r="T7" s="13"/>
+      <c r="S7" s="11"/>
+      <c r="T7" s="11"/>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A8" s="3">
+      <c r="A8" s="12">
         <v>45617</v>
       </c>
       <c r="B8" s="1">
@@ -969,10 +972,10 @@
       <c r="D8" s="1">
         <v>1</v>
       </c>
-      <c r="E8" s="4">
+      <c r="E8" s="3">
         <v>67</v>
       </c>
-      <c r="F8" s="5">
+      <c r="F8" s="4">
         <v>27</v>
       </c>
       <c r="G8" s="1">
@@ -981,10 +984,10 @@
       <c r="H8" s="1">
         <v>249</v>
       </c>
-      <c r="I8" s="13">
+      <c r="I8" s="11">
         <v>1.4</v>
       </c>
-      <c r="J8" s="13">
+      <c r="J8" s="11">
         <v>1.5</v>
       </c>
       <c r="K8" s="1">
@@ -993,25 +996,25 @@
       <c r="L8" s="1">
         <v>229</v>
       </c>
-      <c r="M8" s="6">
-        <v>0</v>
-      </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
-      <c r="O8" s="6">
+      <c r="M8" s="5">
+        <v>0</v>
+      </c>
+      <c r="N8" s="5">
+        <v>0</v>
+      </c>
+      <c r="O8" s="5">
         <v>101</v>
       </c>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11">
+      <c r="P8" s="9"/>
+      <c r="Q8" s="9"/>
+      <c r="R8" s="9">
         <v>66.828000000000003</v>
       </c>
-      <c r="S8" s="13"/>
-      <c r="T8" s="13"/>
+      <c r="S8" s="11"/>
+      <c r="T8" s="11"/>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A9" s="3">
+      <c r="A9" s="12">
         <v>45647</v>
       </c>
       <c r="B9" s="1">
@@ -1023,10 +1026,10 @@
       <c r="D9" s="1">
         <v>1</v>
       </c>
-      <c r="E9" s="4">
+      <c r="E9" s="3">
         <v>66</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F9" s="4">
         <v>27</v>
       </c>
       <c r="G9" s="1">
@@ -1035,10 +1038,10 @@
       <c r="H9" s="1">
         <v>250</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <v>1.4</v>
       </c>
-      <c r="J9" s="13">
+      <c r="J9" s="11">
         <v>2.8</v>
       </c>
       <c r="K9" s="1">
@@ -1047,27 +1050,27 @@
       <c r="L9" s="1">
         <v>220</v>
       </c>
-      <c r="M9" s="6">
-        <v>0</v>
-      </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
-      <c r="O9" s="6">
+      <c r="M9" s="5">
+        <v>0</v>
+      </c>
+      <c r="N9" s="5">
+        <v>0</v>
+      </c>
+      <c r="O9" s="5">
         <v>103</v>
       </c>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11">
+      <c r="P9" s="9"/>
+      <c r="Q9" s="9">
         <v>0.30399999999999999</v>
       </c>
-      <c r="R9" s="11">
+      <c r="R9" s="9">
         <v>66.016000000000005</v>
       </c>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
+      <c r="S9" s="11"/>
+      <c r="T9" s="11"/>
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A10" s="3">
+      <c r="A10" s="12">
         <v>45313</v>
       </c>
       <c r="B10" s="1">
@@ -1079,10 +1082,10 @@
       <c r="D10" s="1">
         <v>1</v>
       </c>
-      <c r="E10" s="4">
+      <c r="E10" s="3">
         <v>67</v>
       </c>
-      <c r="F10" s="5">
+      <c r="F10" s="4">
         <v>28</v>
       </c>
       <c r="G10" s="1">
@@ -1091,10 +1094,10 @@
       <c r="H10" s="1">
         <v>244</v>
       </c>
-      <c r="I10" s="13">
+      <c r="I10" s="11">
         <v>1.3</v>
       </c>
-      <c r="J10" s="13">
+      <c r="J10" s="11">
         <v>2.5</v>
       </c>
       <c r="K10" s="1">
@@ -1103,27 +1106,27 @@
       <c r="L10" s="1">
         <v>217</v>
       </c>
-      <c r="M10" s="6">
-        <v>0</v>
-      </c>
-      <c r="N10" s="6">
+      <c r="M10" s="5">
+        <v>0</v>
+      </c>
+      <c r="N10" s="5">
         <v>1</v>
       </c>
-      <c r="O10" s="6">
+      <c r="O10" s="5">
         <v>99</v>
       </c>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11">
+      <c r="P10" s="9"/>
+      <c r="Q10" s="9">
         <v>1.9219999999999999</v>
       </c>
-      <c r="R10" s="11">
+      <c r="R10" s="9">
         <v>66.468000000000004</v>
       </c>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A11" s="3">
+      <c r="A11" s="12">
         <v>45344</v>
       </c>
       <c r="B11" s="1">
@@ -1135,10 +1138,10 @@
       <c r="D11" s="1">
         <v>1</v>
       </c>
-      <c r="E11" s="4">
+      <c r="E11" s="3">
         <v>67</v>
       </c>
-      <c r="F11" s="5">
+      <c r="F11" s="4">
         <v>27</v>
       </c>
       <c r="G11" s="1">
@@ -1147,10 +1150,10 @@
       <c r="H11" s="1">
         <v>249</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="11">
         <v>1.3</v>
       </c>
-      <c r="J11" s="13">
+      <c r="J11" s="11">
         <v>2.7</v>
       </c>
       <c r="K11" s="1">
@@ -1159,27 +1162,27 @@
       <c r="L11" s="1">
         <v>211</v>
       </c>
-      <c r="M11" s="6">
-        <v>0</v>
-      </c>
-      <c r="N11" s="6">
+      <c r="M11" s="5">
+        <v>0</v>
+      </c>
+      <c r="N11" s="5">
         <v>4</v>
       </c>
-      <c r="O11" s="6">
+      <c r="O11" s="5">
         <v>84</v>
       </c>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11">
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9">
         <v>6.1840000000000002</v>
       </c>
-      <c r="R11" s="11">
+      <c r="R11" s="9">
         <v>64.432000000000002</v>
       </c>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
+      <c r="S11" s="11"/>
+      <c r="T11" s="11"/>
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A12" s="3">
+      <c r="A12" s="12">
         <v>45373</v>
       </c>
       <c r="B12" s="1">
@@ -1191,10 +1194,10 @@
       <c r="D12" s="1">
         <v>1.01</v>
       </c>
-      <c r="E12" s="4">
+      <c r="E12" s="3">
         <v>65</v>
       </c>
-      <c r="F12" s="5">
+      <c r="F12" s="4">
         <v>27</v>
       </c>
       <c r="G12" s="1">
@@ -1203,10 +1206,10 @@
       <c r="H12" s="1">
         <v>240</v>
       </c>
-      <c r="I12" s="13">
+      <c r="I12" s="11">
         <v>1.3</v>
       </c>
-      <c r="J12" s="13">
+      <c r="J12" s="11">
         <v>2.7</v>
       </c>
       <c r="K12" s="1">
@@ -1215,27 +1218,27 @@
       <c r="L12" s="1">
         <v>221</v>
       </c>
-      <c r="M12" s="6">
-        <v>0</v>
-      </c>
-      <c r="N12" s="6">
+      <c r="M12" s="5">
+        <v>0</v>
+      </c>
+      <c r="N12" s="5">
         <v>16</v>
       </c>
-      <c r="O12" s="6">
+      <c r="O12" s="5">
         <v>85</v>
       </c>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11">
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9">
         <v>17.071999999999999</v>
       </c>
-      <c r="R12" s="11">
+      <c r="R12" s="9">
         <v>59.908999999999999</v>
       </c>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
+      <c r="S12" s="11"/>
+      <c r="T12" s="11"/>
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A13" s="3">
+      <c r="A13" s="12">
         <v>45404</v>
       </c>
       <c r="B13" s="1">
@@ -1247,10 +1250,10 @@
       <c r="D13" s="1">
         <v>1.03</v>
       </c>
-      <c r="E13" s="4">
+      <c r="E13" s="3">
         <v>64</v>
       </c>
-      <c r="F13" s="5">
+      <c r="F13" s="4">
         <v>28</v>
       </c>
       <c r="G13" s="1">
@@ -1259,10 +1262,10 @@
       <c r="H13" s="1">
         <v>241</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <v>1.3</v>
       </c>
-      <c r="J13" s="13">
+      <c r="J13" s="11">
         <v>2.7</v>
       </c>
       <c r="K13" s="1">
@@ -1271,27 +1274,27 @@
       <c r="L13" s="1">
         <v>219</v>
       </c>
-      <c r="M13" s="6">
-        <v>0</v>
-      </c>
-      <c r="N13" s="6">
+      <c r="M13" s="5">
+        <v>0</v>
+      </c>
+      <c r="N13" s="5">
         <v>30</v>
       </c>
-      <c r="O13" s="6">
+      <c r="O13" s="5">
         <v>64</v>
       </c>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11">
+      <c r="P13" s="9"/>
+      <c r="Q13" s="9">
         <v>24.654</v>
       </c>
-      <c r="R13" s="11">
+      <c r="R13" s="9">
         <v>49.731000000000002</v>
       </c>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
+      <c r="S13" s="11"/>
+      <c r="T13" s="11"/>
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A14" s="3">
+      <c r="A14" s="12">
         <v>45434</v>
       </c>
       <c r="B14" s="1">
@@ -1303,10 +1306,10 @@
       <c r="D14" s="1">
         <v>1.05</v>
       </c>
-      <c r="E14" s="4">
+      <c r="E14" s="3">
         <v>63</v>
       </c>
-      <c r="F14" s="5">
+      <c r="F14" s="4">
         <v>28</v>
       </c>
       <c r="G14" s="1">
@@ -1315,10 +1318,10 @@
       <c r="H14" s="1">
         <v>249</v>
       </c>
-      <c r="I14" s="13">
+      <c r="I14" s="11">
         <v>1.3</v>
       </c>
-      <c r="J14" s="13">
+      <c r="J14" s="11">
         <v>2.7</v>
       </c>
       <c r="K14" s="1">
@@ -1327,27 +1330,27 @@
       <c r="L14" s="1">
         <v>221</v>
       </c>
-      <c r="M14" s="6">
-        <v>0</v>
-      </c>
-      <c r="N14" s="6">
+      <c r="M14" s="5">
+        <v>0</v>
+      </c>
+      <c r="N14" s="5">
         <v>49</v>
       </c>
-      <c r="O14" s="6">
+      <c r="O14" s="5">
         <v>48</v>
       </c>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11">
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9">
         <v>34.317999999999998</v>
       </c>
-      <c r="R14" s="11">
+      <c r="R14" s="9">
         <v>41.542000000000002</v>
       </c>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A15" s="3">
+      <c r="A15" s="12">
         <v>45465</v>
       </c>
       <c r="B15" s="1">
@@ -1359,10 +1362,10 @@
       <c r="D15" s="1">
         <v>1.07</v>
       </c>
-      <c r="E15" s="4">
+      <c r="E15" s="3">
         <v>62</v>
       </c>
-      <c r="F15" s="5">
+      <c r="F15" s="4">
         <v>27</v>
       </c>
       <c r="G15" s="1">
@@ -1371,10 +1374,10 @@
       <c r="H15" s="1">
         <v>246</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="11">
         <v>1.3</v>
       </c>
-      <c r="J15" s="13">
+      <c r="J15" s="11">
         <v>2.7</v>
       </c>
       <c r="K15" s="1">
@@ -1383,27 +1386,27 @@
       <c r="L15" s="1">
         <v>221</v>
       </c>
-      <c r="M15" s="6">
-        <v>0</v>
-      </c>
-      <c r="N15" s="6">
+      <c r="M15" s="5">
+        <v>0</v>
+      </c>
+      <c r="N15" s="5">
         <v>62</v>
       </c>
-      <c r="O15" s="6">
+      <c r="O15" s="5">
         <v>28</v>
       </c>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11">
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9">
         <v>41.177999999999997</v>
       </c>
-      <c r="R15" s="11">
+      <c r="R15" s="9">
         <v>32.692999999999998</v>
       </c>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
+      <c r="S15" s="11"/>
+      <c r="T15" s="11"/>
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A16" s="3">
+      <c r="A16" s="12">
         <v>45495</v>
       </c>
       <c r="B16" s="1">
@@ -1415,10 +1418,10 @@
       <c r="D16" s="1">
         <v>1.0900000000000001</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>63</v>
       </c>
-      <c r="F16" s="5">
+      <c r="F16" s="4">
         <v>27</v>
       </c>
       <c r="G16" s="1">
@@ -1427,10 +1430,10 @@
       <c r="H16" s="1">
         <v>238</v>
       </c>
-      <c r="I16" s="13">
+      <c r="I16" s="11">
         <v>1.3</v>
       </c>
-      <c r="J16" s="13">
+      <c r="J16" s="11">
         <v>2.7</v>
       </c>
       <c r="K16" s="1">
@@ -1439,27 +1442,27 @@
       <c r="L16" s="1">
         <v>204</v>
       </c>
-      <c r="M16" s="6">
-        <v>0</v>
-      </c>
-      <c r="N16" s="6">
+      <c r="M16" s="5">
+        <v>0</v>
+      </c>
+      <c r="N16" s="5">
         <v>71</v>
       </c>
-      <c r="O16" s="6">
+      <c r="O16" s="5">
         <v>20</v>
       </c>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11">
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9">
         <v>47.91</v>
       </c>
-      <c r="R16" s="11">
+      <c r="R16" s="9">
         <v>24.728999999999999</v>
       </c>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
+      <c r="S16" s="11"/>
+      <c r="T16" s="11"/>
     </row>
     <row r="17" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A17" s="3">
+      <c r="A17" s="12">
         <v>45526</v>
       </c>
       <c r="B17" s="1">
@@ -1471,10 +1474,10 @@
       <c r="D17" s="1">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E17" s="4">
+      <c r="E17" s="3">
         <v>62</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>26</v>
       </c>
       <c r="G17" s="1">
@@ -1483,10 +1486,10 @@
       <c r="H17" s="1">
         <v>238</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="11">
         <v>1.3</v>
       </c>
-      <c r="J17" s="13">
+      <c r="J17" s="11">
         <v>2.7</v>
       </c>
       <c r="K17" s="1">
@@ -1495,27 +1498,27 @@
       <c r="L17" s="1">
         <v>203</v>
       </c>
-      <c r="M17" s="6">
-        <v>0</v>
-      </c>
-      <c r="N17" s="6">
+      <c r="M17" s="5">
+        <v>0</v>
+      </c>
+      <c r="N17" s="5">
         <v>74</v>
       </c>
-      <c r="O17" s="6">
+      <c r="O17" s="5">
         <v>13</v>
       </c>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11">
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9">
         <v>50.552</v>
       </c>
-      <c r="R17" s="11">
+      <c r="R17" s="9">
         <v>19.721</v>
       </c>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
+      <c r="S17" s="11"/>
+      <c r="T17" s="11"/>
     </row>
     <row r="18" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A18" s="3">
+      <c r="A18" s="12">
         <v>45557</v>
       </c>
       <c r="B18" s="1">
@@ -1527,10 +1530,10 @@
       <c r="D18" s="1">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="3">
         <v>61</v>
       </c>
-      <c r="F18" s="5">
+      <c r="F18" s="4">
         <v>25</v>
       </c>
       <c r="G18" s="1">
@@ -1539,10 +1542,10 @@
       <c r="H18" s="1">
         <v>235</v>
       </c>
-      <c r="I18" s="13">
+      <c r="I18" s="11">
         <v>1.3</v>
       </c>
-      <c r="J18" s="13">
+      <c r="J18" s="11">
         <v>2.7</v>
       </c>
       <c r="K18" s="1">
@@ -1551,27 +1554,27 @@
       <c r="L18" s="1">
         <v>184</v>
       </c>
-      <c r="M18" s="6">
-        <v>0</v>
-      </c>
-      <c r="N18" s="6">
+      <c r="M18" s="5">
+        <v>0</v>
+      </c>
+      <c r="N18" s="5">
         <v>78</v>
       </c>
-      <c r="O18" s="6">
+      <c r="O18" s="5">
         <v>9</v>
       </c>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11">
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9">
         <v>51.738</v>
       </c>
-      <c r="R18" s="11">
+      <c r="R18" s="9">
         <v>14.818</v>
       </c>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
+      <c r="S18" s="11"/>
+      <c r="T18" s="11"/>
     </row>
     <row r="19" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A19" s="3">
+      <c r="A19" s="12">
         <v>45587</v>
       </c>
       <c r="B19" s="1">
@@ -1583,10 +1586,10 @@
       <c r="D19" s="1">
         <v>1.1100000000000001</v>
       </c>
-      <c r="E19" s="4">
+      <c r="E19" s="3">
         <v>61</v>
       </c>
-      <c r="F19" s="5">
+      <c r="F19" s="4">
         <v>24</v>
       </c>
       <c r="G19" s="1">
@@ -1595,10 +1598,10 @@
       <c r="H19" s="1">
         <v>239</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="11">
         <v>1.3</v>
       </c>
-      <c r="J19" s="13">
+      <c r="J19" s="11">
         <v>2.7</v>
       </c>
       <c r="K19" s="1">
@@ -1607,27 +1610,27 @@
       <c r="L19" s="1">
         <v>182</v>
       </c>
-      <c r="M19" s="6">
-        <v>0</v>
-      </c>
-      <c r="N19" s="6">
+      <c r="M19" s="5">
+        <v>0</v>
+      </c>
+      <c r="N19" s="5">
         <v>80</v>
       </c>
-      <c r="O19" s="6">
+      <c r="O19" s="5">
         <v>7</v>
       </c>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11">
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9">
         <v>53.167000000000002</v>
       </c>
-      <c r="R19" s="11">
+      <c r="R19" s="9">
         <v>10.99</v>
       </c>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
+      <c r="S19" s="11"/>
+      <c r="T19" s="11"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A20" s="3">
+      <c r="A20" s="12">
         <v>45618</v>
       </c>
       <c r="B20" s="1">
@@ -1639,10 +1642,10 @@
       <c r="D20" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E20" s="4">
+      <c r="E20" s="3">
         <v>61</v>
       </c>
-      <c r="F20" s="5">
+      <c r="F20" s="4">
         <v>26</v>
       </c>
       <c r="G20" s="1">
@@ -1651,10 +1654,10 @@
       <c r="H20" s="1">
         <v>244</v>
       </c>
-      <c r="I20" s="13">
+      <c r="I20" s="11">
         <v>1.3</v>
       </c>
-      <c r="J20" s="13">
+      <c r="J20" s="11">
         <v>2.7</v>
       </c>
       <c r="K20" s="1">
@@ -1663,27 +1666,27 @@
       <c r="L20" s="1">
         <v>177</v>
       </c>
-      <c r="M20" s="6">
-        <v>0</v>
-      </c>
-      <c r="N20" s="6">
+      <c r="M20" s="5">
+        <v>0</v>
+      </c>
+      <c r="N20" s="5">
         <v>82</v>
       </c>
-      <c r="O20" s="6">
+      <c r="O20" s="5">
         <v>7</v>
       </c>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11">
+      <c r="P20" s="9"/>
+      <c r="Q20" s="9">
         <v>54.042999999999999</v>
       </c>
-      <c r="R20" s="11">
+      <c r="R20" s="9">
         <v>10.68</v>
       </c>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
+      <c r="S20" s="11"/>
+      <c r="T20" s="11"/>
     </row>
     <row r="21" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A21" s="3">
+      <c r="A21" s="12">
         <v>45648</v>
       </c>
       <c r="B21" s="1">
@@ -1695,10 +1698,10 @@
       <c r="D21" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E21" s="4">
+      <c r="E21" s="3">
         <v>62</v>
       </c>
-      <c r="F21" s="5">
+      <c r="F21" s="4">
         <v>26</v>
       </c>
       <c r="G21" s="1">
@@ -1707,10 +1710,10 @@
       <c r="H21" s="1">
         <v>251</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I21" s="11">
         <v>1.3</v>
       </c>
-      <c r="J21" s="13">
+      <c r="J21" s="11">
         <v>2.7</v>
       </c>
       <c r="K21" s="1">
@@ -1719,27 +1722,27 @@
       <c r="L21" s="1">
         <v>187</v>
       </c>
-      <c r="M21" s="6">
-        <v>0</v>
-      </c>
-      <c r="N21" s="6">
+      <c r="M21" s="5">
+        <v>0</v>
+      </c>
+      <c r="N21" s="5">
         <v>84</v>
       </c>
-      <c r="O21" s="6">
+      <c r="O21" s="5">
         <v>6</v>
       </c>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11">
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9">
         <v>56.247</v>
       </c>
-      <c r="R21" s="11">
+      <c r="R21" s="9">
         <v>9.0220000000000002</v>
       </c>
-      <c r="S21" s="13"/>
-      <c r="T21" s="13"/>
+      <c r="S21" s="11"/>
+      <c r="T21" s="11"/>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A22" s="3">
+      <c r="A22" s="12">
         <v>45314</v>
       </c>
       <c r="B22" s="1">
@@ -1751,10 +1754,10 @@
       <c r="D22" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E22" s="4">
+      <c r="E22" s="3">
         <v>61</v>
       </c>
-      <c r="F22" s="5">
+      <c r="F22" s="4">
         <v>28</v>
       </c>
       <c r="G22" s="1">
@@ -1763,10 +1766,10 @@
       <c r="H22" s="1">
         <v>262</v>
       </c>
-      <c r="I22" s="13">
+      <c r="I22" s="11">
         <v>1.3</v>
       </c>
-      <c r="J22" s="13">
+      <c r="J22" s="11">
         <v>2.7</v>
       </c>
       <c r="K22" s="1">
@@ -1775,27 +1778,27 @@
       <c r="L22" s="1">
         <v>172</v>
       </c>
-      <c r="M22" s="6">
-        <v>0</v>
-      </c>
-      <c r="N22" s="6">
+      <c r="M22" s="5">
+        <v>0</v>
+      </c>
+      <c r="N22" s="5">
         <v>89</v>
       </c>
-      <c r="O22" s="6">
+      <c r="O22" s="5">
         <v>4</v>
       </c>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11">
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9">
         <v>57.466000000000001</v>
       </c>
-      <c r="R22" s="11">
+      <c r="R22" s="9">
         <v>6.4059999999999997</v>
       </c>
-      <c r="S22" s="13"/>
-      <c r="T22" s="13"/>
+      <c r="S22" s="11"/>
+      <c r="T22" s="11"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A23" s="3">
+      <c r="A23" s="12">
         <v>45345</v>
       </c>
       <c r="B23" s="1">
@@ -1807,10 +1810,10 @@
       <c r="D23" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E23" s="4">
+      <c r="E23" s="3">
         <v>61</v>
       </c>
-      <c r="F23" s="5">
+      <c r="F23" s="4">
         <v>31</v>
       </c>
       <c r="G23" s="1">
@@ -1819,10 +1822,10 @@
       <c r="H23" s="1">
         <v>264</v>
       </c>
-      <c r="I23" s="13">
+      <c r="I23" s="11">
         <v>1.3</v>
       </c>
-      <c r="J23" s="13">
+      <c r="J23" s="11">
         <v>2.7</v>
       </c>
       <c r="K23" s="1">
@@ -1831,27 +1834,27 @@
       <c r="L23" s="1">
         <v>163</v>
       </c>
-      <c r="M23" s="6">
-        <v>0</v>
-      </c>
-      <c r="N23" s="6">
+      <c r="M23" s="5">
+        <v>0</v>
+      </c>
+      <c r="N23" s="5">
         <v>83</v>
       </c>
-      <c r="O23" s="6">
+      <c r="O23" s="5">
         <v>4</v>
       </c>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11">
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9">
         <v>57.793999999999997</v>
       </c>
-      <c r="R23" s="11">
+      <c r="R23" s="9">
         <v>5.6449999999999996</v>
       </c>
-      <c r="S23" s="13"/>
-      <c r="T23" s="13"/>
+      <c r="S23" s="11"/>
+      <c r="T23" s="11"/>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A24" s="3">
+      <c r="A24" s="12">
         <v>45374</v>
       </c>
       <c r="B24" s="1">
@@ -1863,10 +1866,10 @@
       <c r="D24" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E24" s="4">
+      <c r="E24" s="3">
         <v>61</v>
       </c>
-      <c r="F24" s="5">
+      <c r="F24" s="4">
         <v>30</v>
       </c>
       <c r="G24" s="1">
@@ -1875,10 +1878,10 @@
       <c r="H24" s="1">
         <v>267</v>
       </c>
-      <c r="I24" s="13">
+      <c r="I24" s="11">
         <v>1.3</v>
       </c>
-      <c r="J24" s="13">
+      <c r="J24" s="11">
         <v>2.7</v>
       </c>
       <c r="K24" s="1">
@@ -1887,27 +1890,27 @@
       <c r="L24" s="1">
         <v>207</v>
       </c>
-      <c r="M24" s="6">
-        <v>0</v>
-      </c>
-      <c r="N24" s="6">
+      <c r="M24" s="5">
+        <v>0</v>
+      </c>
+      <c r="N24" s="5">
         <v>90</v>
       </c>
-      <c r="O24" s="6">
+      <c r="O24" s="5">
         <v>3</v>
       </c>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11">
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9">
         <v>57.06</v>
       </c>
-      <c r="R24" s="11">
+      <c r="R24" s="9">
         <v>5.641</v>
       </c>
-      <c r="S24" s="13"/>
-      <c r="T24" s="13"/>
+      <c r="S24" s="11"/>
+      <c r="T24" s="11"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A25" s="3">
+      <c r="A25" s="12">
         <v>45405</v>
       </c>
       <c r="B25" s="1">
@@ -1919,10 +1922,10 @@
       <c r="D25" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E25" s="4">
+      <c r="E25" s="3">
         <v>61</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F25" s="4">
         <v>31</v>
       </c>
       <c r="G25" s="1">
@@ -1931,10 +1934,10 @@
       <c r="H25" s="1">
         <v>267</v>
       </c>
-      <c r="I25" s="13">
+      <c r="I25" s="11">
         <v>1.3</v>
       </c>
-      <c r="J25" s="13">
+      <c r="J25" s="11">
         <v>2.7</v>
       </c>
       <c r="K25" s="1">
@@ -1943,27 +1946,27 @@
       <c r="L25" s="1">
         <v>196</v>
       </c>
-      <c r="M25" s="6">
-        <v>0</v>
-      </c>
-      <c r="N25" s="6">
+      <c r="M25" s="5">
+        <v>0</v>
+      </c>
+      <c r="N25" s="5">
         <v>92</v>
       </c>
-      <c r="O25" s="6">
+      <c r="O25" s="5">
         <v>3</v>
       </c>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11">
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9">
         <v>57.752000000000002</v>
       </c>
-      <c r="R25" s="11">
+      <c r="R25" s="9">
         <v>3.9969999999999999</v>
       </c>
-      <c r="S25" s="13"/>
-      <c r="T25" s="13"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
     </row>
     <row r="26" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A26" s="3">
+      <c r="A26" s="12">
         <v>45435</v>
       </c>
       <c r="B26" s="1">
@@ -1975,10 +1978,10 @@
       <c r="D26" s="1">
         <v>1.1200000000000001</v>
       </c>
-      <c r="E26" s="4">
+      <c r="E26" s="3">
         <v>60</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F26" s="4">
         <v>31</v>
       </c>
       <c r="G26" s="1">
@@ -1987,10 +1990,10 @@
       <c r="H26" s="1">
         <v>266</v>
       </c>
-      <c r="I26" s="13">
+      <c r="I26" s="11">
         <v>1.3</v>
       </c>
-      <c r="J26" s="13">
+      <c r="J26" s="11">
         <v>2.7</v>
       </c>
       <c r="K26" s="1">
@@ -1999,27 +2002,27 @@
       <c r="L26" s="1">
         <v>206</v>
       </c>
-      <c r="M26" s="6">
-        <v>0</v>
-      </c>
-      <c r="N26" s="6">
+      <c r="M26" s="5">
+        <v>0</v>
+      </c>
+      <c r="N26" s="5">
         <v>93</v>
       </c>
-      <c r="O26" s="6">
+      <c r="O26" s="5">
         <v>3</v>
       </c>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11">
+      <c r="P26" s="9"/>
+      <c r="Q26" s="9">
         <v>56.668999999999997</v>
       </c>
-      <c r="R26" s="11">
+      <c r="R26" s="9">
         <v>4.1929999999999996</v>
       </c>
-      <c r="S26" s="13"/>
-      <c r="T26" s="13"/>
+      <c r="S26" s="11"/>
+      <c r="T26" s="11"/>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A27" s="3">
+      <c r="A27" s="12">
         <v>45466</v>
       </c>
       <c r="B27" s="1">
@@ -2031,10 +2034,10 @@
       <c r="D27" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E27" s="4">
+      <c r="E27" s="3">
         <v>58</v>
       </c>
-      <c r="F27" s="5">
+      <c r="F27" s="4">
         <v>31</v>
       </c>
       <c r="G27" s="1">
@@ -2043,10 +2046,10 @@
       <c r="H27" s="1">
         <v>274</v>
       </c>
-      <c r="I27" s="13">
+      <c r="I27" s="11">
         <v>1.3</v>
       </c>
-      <c r="J27" s="13">
+      <c r="J27" s="11">
         <v>2.7</v>
       </c>
       <c r="K27" s="1">
@@ -2055,27 +2058,27 @@
       <c r="L27" s="1">
         <v>181</v>
       </c>
-      <c r="M27" s="6">
-        <v>0</v>
-      </c>
-      <c r="N27" s="6">
+      <c r="M27" s="5">
+        <v>0</v>
+      </c>
+      <c r="N27" s="5">
         <v>91</v>
       </c>
-      <c r="O27" s="6">
+      <c r="O27" s="5">
         <v>2</v>
       </c>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11">
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9">
         <v>55.311</v>
       </c>
-      <c r="R27" s="11">
+      <c r="R27" s="9">
         <v>3.6560000000000001</v>
       </c>
-      <c r="S27" s="13"/>
-      <c r="T27" s="13"/>
+      <c r="S27" s="11"/>
+      <c r="T27" s="11"/>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A28" s="3">
+      <c r="A28" s="12">
         <v>45496</v>
       </c>
       <c r="B28" s="1">
@@ -2087,10 +2090,10 @@
       <c r="D28" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E28" s="4">
+      <c r="E28" s="3">
         <v>58</v>
       </c>
-      <c r="F28" s="5">
+      <c r="F28" s="4">
         <v>31</v>
       </c>
       <c r="G28" s="1">
@@ -2099,10 +2102,10 @@
       <c r="H28" s="1">
         <v>279</v>
       </c>
-      <c r="I28" s="13">
+      <c r="I28" s="11">
         <v>1.3</v>
       </c>
-      <c r="J28" s="13">
+      <c r="J28" s="11">
         <v>2.7</v>
       </c>
       <c r="K28" s="1">
@@ -2111,27 +2114,27 @@
       <c r="L28" s="1">
         <v>179</v>
       </c>
-      <c r="M28" s="6">
-        <v>0</v>
-      </c>
-      <c r="N28" s="6">
+      <c r="M28" s="5">
+        <v>0</v>
+      </c>
+      <c r="N28" s="5">
         <v>92</v>
       </c>
-      <c r="O28" s="6">
+      <c r="O28" s="5">
         <v>2</v>
       </c>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11">
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9">
         <v>56.194000000000003</v>
       </c>
-      <c r="R28" s="11">
+      <c r="R28" s="9">
         <v>2.39</v>
       </c>
-      <c r="S28" s="13"/>
-      <c r="T28" s="13"/>
+      <c r="S28" s="11"/>
+      <c r="T28" s="11"/>
     </row>
     <row r="29" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A29" s="3">
+      <c r="A29" s="12">
         <v>45527</v>
       </c>
       <c r="B29" s="1">
@@ -2143,10 +2146,10 @@
       <c r="D29" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E29" s="4">
+      <c r="E29" s="3">
         <v>59</v>
       </c>
-      <c r="F29" s="5">
+      <c r="F29" s="4">
         <v>33</v>
       </c>
       <c r="G29" s="1">
@@ -2155,10 +2158,10 @@
       <c r="H29" s="1">
         <v>277</v>
       </c>
-      <c r="I29" s="13">
+      <c r="I29" s="11">
         <v>1.5</v>
       </c>
-      <c r="J29" s="13">
+      <c r="J29" s="11">
         <v>2.7</v>
       </c>
       <c r="K29" s="1">
@@ -2167,27 +2170,27 @@
       <c r="L29" s="1">
         <v>174</v>
       </c>
-      <c r="M29" s="6">
-        <v>0</v>
-      </c>
-      <c r="N29" s="6">
+      <c r="M29" s="5">
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
         <v>90</v>
       </c>
-      <c r="O29" s="6">
+      <c r="O29" s="5">
         <v>2</v>
       </c>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11">
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9">
         <v>57.371000000000002</v>
       </c>
-      <c r="R29" s="11">
+      <c r="R29" s="9">
         <v>2.0259999999999998</v>
       </c>
-      <c r="S29" s="13"/>
-      <c r="T29" s="13"/>
+      <c r="S29" s="11"/>
+      <c r="T29" s="11"/>
     </row>
     <row r="30" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A30" s="3">
+      <c r="A30" s="12">
         <v>45558</v>
       </c>
       <c r="B30" s="1">
@@ -2199,10 +2202,10 @@
       <c r="D30" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E30" s="4">
+      <c r="E30" s="3">
         <v>59</v>
       </c>
-      <c r="F30" s="5">
+      <c r="F30" s="4">
         <v>37</v>
       </c>
       <c r="G30" s="1">
@@ -2211,10 +2214,10 @@
       <c r="H30" s="1">
         <v>283</v>
       </c>
-      <c r="I30" s="13">
+      <c r="I30" s="11">
         <v>1.5</v>
       </c>
-      <c r="J30" s="13">
+      <c r="J30" s="11">
         <v>2.5</v>
       </c>
       <c r="K30" s="1">
@@ -2223,27 +2226,27 @@
       <c r="L30" s="1">
         <v>174</v>
       </c>
-      <c r="M30" s="6">
-        <v>0</v>
-      </c>
-      <c r="N30" s="6">
+      <c r="M30" s="5">
+        <v>0</v>
+      </c>
+      <c r="N30" s="5">
         <v>92</v>
       </c>
-      <c r="O30" s="6">
+      <c r="O30" s="5">
         <v>2</v>
       </c>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11">
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9">
         <v>57.482999999999997</v>
       </c>
-      <c r="R30" s="11">
+      <c r="R30" s="9">
         <v>1.7669999999999999</v>
       </c>
-      <c r="S30" s="13"/>
-      <c r="T30" s="13"/>
+      <c r="S30" s="11"/>
+      <c r="T30" s="11"/>
     </row>
     <row r="31" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A31" s="3">
+      <c r="A31" s="12">
         <v>45588</v>
       </c>
       <c r="B31" s="1">
@@ -2255,10 +2258,10 @@
       <c r="D31" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E31" s="4">
+      <c r="E31" s="3">
         <v>59</v>
       </c>
-      <c r="F31" s="5">
+      <c r="F31" s="4">
         <v>37</v>
       </c>
       <c r="G31" s="1">
@@ -2267,10 +2270,10 @@
       <c r="H31" s="1">
         <v>282</v>
       </c>
-      <c r="I31" s="13">
+      <c r="I31" s="11">
         <v>1.5</v>
       </c>
-      <c r="J31" s="13">
+      <c r="J31" s="11">
         <v>2.5</v>
       </c>
       <c r="K31" s="1">
@@ -2279,27 +2282,27 @@
       <c r="L31" s="1">
         <v>159</v>
       </c>
-      <c r="M31" s="6">
-        <v>0</v>
-      </c>
-      <c r="N31" s="6">
+      <c r="M31" s="5">
+        <v>0</v>
+      </c>
+      <c r="N31" s="5">
         <v>96</v>
       </c>
-      <c r="O31" s="6">
+      <c r="O31" s="5">
         <v>2</v>
       </c>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11">
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9">
         <v>57.244999999999997</v>
       </c>
-      <c r="R31" s="11">
+      <c r="R31" s="9">
         <v>1.788</v>
       </c>
-      <c r="S31" s="13"/>
-      <c r="T31" s="13"/>
+      <c r="S31" s="11"/>
+      <c r="T31" s="11"/>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A32" s="3">
+      <c r="A32" s="12">
         <v>45619</v>
       </c>
       <c r="B32" s="1">
@@ -2311,10 +2314,10 @@
       <c r="D32" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E32" s="4">
+      <c r="E32" s="3">
         <v>57</v>
       </c>
-      <c r="F32" s="5">
+      <c r="F32" s="4">
         <v>35</v>
       </c>
       <c r="G32" s="1">
@@ -2323,10 +2326,10 @@
       <c r="H32" s="1">
         <v>284</v>
       </c>
-      <c r="I32" s="13">
+      <c r="I32" s="11">
         <v>1.5</v>
       </c>
-      <c r="J32" s="13">
+      <c r="J32" s="11">
         <v>2.5</v>
       </c>
       <c r="K32" s="1">
@@ -2335,29 +2338,29 @@
       <c r="L32" s="1">
         <v>179</v>
       </c>
-      <c r="M32" s="6">
-        <v>0</v>
-      </c>
-      <c r="N32" s="6">
+      <c r="M32" s="5">
+        <v>0</v>
+      </c>
+      <c r="N32" s="5">
         <v>96</v>
       </c>
-      <c r="O32" s="6">
+      <c r="O32" s="5">
         <v>1</v>
       </c>
-      <c r="P32" s="11">
+      <c r="P32" s="9">
         <v>0.32900000000000001</v>
       </c>
-      <c r="Q32" s="11">
+      <c r="Q32" s="9">
         <v>55.018999999999998</v>
       </c>
-      <c r="R32" s="11">
+      <c r="R32" s="9">
         <v>1.9279999999999999</v>
       </c>
-      <c r="S32" s="13"/>
-      <c r="T32" s="13"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A33" s="7">
+      <c r="A33" s="13">
         <v>45649</v>
       </c>
       <c r="B33" s="1">
@@ -2369,10 +2372,10 @@
       <c r="D33" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E33" s="8">
+      <c r="E33" s="6">
         <v>57</v>
       </c>
-      <c r="F33" s="9">
+      <c r="F33" s="7">
         <v>35</v>
       </c>
       <c r="G33" s="1">
@@ -2381,10 +2384,10 @@
       <c r="H33" s="1">
         <v>284</v>
       </c>
-      <c r="I33" s="13">
+      <c r="I33" s="11">
         <v>1.5</v>
       </c>
-      <c r="J33" s="13">
+      <c r="J33" s="11">
         <v>2.5</v>
       </c>
       <c r="K33" s="1">
@@ -2393,29 +2396,29 @@
       <c r="L33" s="1">
         <v>177</v>
       </c>
-      <c r="M33" s="6">
+      <c r="M33" s="5">
         <v>1</v>
       </c>
-      <c r="N33" s="6">
+      <c r="N33" s="5">
         <v>98</v>
       </c>
-      <c r="O33" s="6">
+      <c r="O33" s="5">
         <v>2</v>
       </c>
-      <c r="P33" s="11">
+      <c r="P33" s="9">
         <v>1.3180000000000001</v>
       </c>
-      <c r="Q33" s="11">
+      <c r="Q33" s="9">
         <v>54.863999999999997</v>
       </c>
-      <c r="R33" s="11">
+      <c r="R33" s="9">
         <v>1.6359999999999999</v>
       </c>
-      <c r="S33" s="13"/>
-      <c r="T33" s="13"/>
+      <c r="S33" s="11"/>
+      <c r="T33" s="11"/>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A34" s="3">
+      <c r="A34" s="12">
         <v>45315</v>
       </c>
       <c r="B34" s="1">
@@ -2427,10 +2430,10 @@
       <c r="D34" s="1">
         <v>1.1299999999999999</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="3">
         <v>56</v>
       </c>
-      <c r="F34" s="5">
+      <c r="F34" s="4">
         <v>36</v>
       </c>
       <c r="G34" s="1">
@@ -2439,10 +2442,10 @@
       <c r="H34" s="1">
         <v>283</v>
       </c>
-      <c r="I34" s="13">
+      <c r="I34" s="11">
         <v>1.5</v>
       </c>
-      <c r="J34" s="13">
+      <c r="J34" s="11">
         <v>2.5</v>
       </c>
       <c r="K34" s="1">
@@ -2451,29 +2454,29 @@
       <c r="L34" s="1">
         <v>157</v>
       </c>
-      <c r="M34" s="6">
+      <c r="M34" s="5">
         <v>3</v>
       </c>
-      <c r="N34" s="6">
+      <c r="N34" s="5">
         <v>96</v>
       </c>
-      <c r="O34" s="6">
+      <c r="O34" s="5">
         <v>2</v>
       </c>
-      <c r="P34" s="11">
+      <c r="P34" s="9">
         <v>4.9710000000000001</v>
       </c>
-      <c r="Q34" s="11">
+      <c r="Q34" s="9">
         <v>53.457999999999998</v>
       </c>
-      <c r="R34" s="11">
+      <c r="R34" s="9">
         <v>1.38</v>
       </c>
-      <c r="S34" s="13"/>
-      <c r="T34" s="13"/>
+      <c r="S34" s="11"/>
+      <c r="T34" s="11"/>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A35" s="3">
+      <c r="A35" s="12">
         <v>45346</v>
       </c>
       <c r="B35" s="1">
@@ -2485,10 +2488,10 @@
       <c r="D35" s="1">
         <v>1.1399999999999999</v>
       </c>
-      <c r="E35" s="4">
+      <c r="E35" s="3">
         <v>56</v>
       </c>
-      <c r="F35" s="5">
+      <c r="F35" s="4">
         <v>36</v>
       </c>
       <c r="G35" s="1">
@@ -2497,10 +2500,10 @@
       <c r="H35" s="1">
         <v>280</v>
       </c>
-      <c r="I35" s="13">
+      <c r="I35" s="11">
         <v>1.5</v>
       </c>
-      <c r="J35" s="13">
+      <c r="J35" s="11">
         <v>2.5</v>
       </c>
       <c r="K35" s="1">
@@ -2509,29 +2512,29 @@
       <c r="L35" s="1">
         <v>153</v>
       </c>
-      <c r="M35" s="6">
+      <c r="M35" s="5">
         <v>14</v>
       </c>
-      <c r="N35" s="6">
+      <c r="N35" s="5">
         <v>83</v>
       </c>
-      <c r="O35" s="6">
+      <c r="O35" s="5">
         <v>1</v>
       </c>
-      <c r="P35" s="11">
+      <c r="P35" s="9">
         <v>12.425000000000001</v>
       </c>
-      <c r="Q35" s="11">
+      <c r="Q35" s="9">
         <v>51.12</v>
       </c>
-      <c r="R35" s="11">
+      <c r="R35" s="9">
         <v>1.0840000000000001</v>
       </c>
-      <c r="S35" s="13"/>
-      <c r="T35" s="13"/>
+      <c r="S35" s="11"/>
+      <c r="T35" s="11"/>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A36" s="3">
+      <c r="A36" s="12">
         <v>45375</v>
       </c>
       <c r="B36" s="1">
@@ -2543,10 +2546,10 @@
       <c r="D36" s="1">
         <v>1.1399999999999999</v>
       </c>
-      <c r="E36" s="4">
+      <c r="E36" s="3">
         <v>56</v>
       </c>
-      <c r="F36" s="5">
+      <c r="F36" s="4">
         <v>34</v>
       </c>
       <c r="G36" s="1">
@@ -2555,10 +2558,10 @@
       <c r="H36" s="1">
         <v>277</v>
       </c>
-      <c r="I36" s="13">
+      <c r="I36" s="11">
         <v>1.5</v>
       </c>
-      <c r="J36" s="13">
+      <c r="J36" s="11">
         <v>2.8</v>
       </c>
       <c r="K36" s="1">
@@ -2567,29 +2570,29 @@
       <c r="L36" s="1">
         <v>153</v>
       </c>
-      <c r="M36" s="6">
+      <c r="M36" s="5">
         <v>33</v>
       </c>
-      <c r="N36" s="6">
+      <c r="N36" s="5">
         <v>69</v>
       </c>
-      <c r="O36" s="6">
+      <c r="O36" s="5">
         <v>1</v>
       </c>
-      <c r="P36" s="11">
+      <c r="P36" s="9">
         <v>22.245000000000001</v>
       </c>
-      <c r="Q36" s="11">
+      <c r="Q36" s="9">
         <v>43.55</v>
       </c>
-      <c r="R36" s="11">
+      <c r="R36" s="9">
         <v>1.0429999999999999</v>
       </c>
-      <c r="S36" s="13"/>
-      <c r="T36" s="13"/>
+      <c r="S36" s="11"/>
+      <c r="T36" s="11"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A37" s="3">
+      <c r="A37" s="12">
         <v>45406</v>
       </c>
       <c r="B37" s="1">
@@ -2601,10 +2604,10 @@
       <c r="D37" s="1">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E37" s="4">
+      <c r="E37" s="3">
         <v>56</v>
       </c>
-      <c r="F37" s="5">
+      <c r="F37" s="4">
         <v>33</v>
       </c>
       <c r="G37" s="1">
@@ -2613,10 +2616,10 @@
       <c r="H37" s="1">
         <v>273</v>
       </c>
-      <c r="I37" s="13">
+      <c r="I37" s="11">
         <v>1.5</v>
       </c>
-      <c r="J37" s="13">
+      <c r="J37" s="11">
         <v>2.8</v>
       </c>
       <c r="K37" s="1">
@@ -2625,29 +2628,29 @@
       <c r="L37" s="1">
         <v>153</v>
       </c>
-      <c r="M37" s="6">
+      <c r="M37" s="5">
         <v>42</v>
       </c>
-      <c r="N37" s="6">
+      <c r="N37" s="5">
         <v>53</v>
       </c>
-      <c r="O37" s="6">
-        <v>0</v>
-      </c>
-      <c r="P37" s="11">
+      <c r="O37" s="5">
+        <v>0</v>
+      </c>
+      <c r="P37" s="9">
         <v>29.922000000000001</v>
       </c>
-      <c r="Q37" s="11">
+      <c r="Q37" s="9">
         <v>34.601999999999997</v>
       </c>
-      <c r="R37" s="11">
+      <c r="R37" s="9">
         <v>1.0660000000000001</v>
       </c>
-      <c r="S37" s="13"/>
-      <c r="T37" s="13"/>
+      <c r="S37" s="11"/>
+      <c r="T37" s="11"/>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.2">
-      <c r="A38" s="3">
+      <c r="A38" s="12">
         <v>45436</v>
       </c>
       <c r="B38" s="1">
@@ -2659,10 +2662,10 @@
       <c r="D38" s="1">
         <v>1.1499999999999999</v>
       </c>
-      <c r="E38" s="4">
+      <c r="E38" s="3">
         <v>56</v>
       </c>
-      <c r="F38" s="5">
+      <c r="F38" s="4">
         <v>33</v>
       </c>
       <c r="G38" s="1">
@@ -2671,10 +2674,10 @@
       <c r="H38" s="1">
         <v>269</v>
       </c>
-      <c r="I38" s="13">
+      <c r="I38" s="11">
         <v>1.5</v>
       </c>
-      <c r="J38" s="13">
+      <c r="J38" s="11">
         <v>2.8</v>
       </c>
       <c r="K38" s="1">
@@ -2683,26 +2686,26 @@
       <c r="L38" s="1">
         <v>172</v>
       </c>
-      <c r="M38" s="6">
+      <c r="M38" s="5">
         <v>54</v>
       </c>
-      <c r="N38" s="6">
+      <c r="N38" s="5">
         <v>36</v>
       </c>
-      <c r="O38" s="6">
-        <v>0</v>
-      </c>
-      <c r="P38" s="11">
+      <c r="O38" s="5">
+        <v>0</v>
+      </c>
+      <c r="P38" s="9">
         <v>35.908999999999999</v>
       </c>
-      <c r="Q38" s="11">
+      <c r="Q38" s="9">
         <v>27.544</v>
       </c>
-      <c r="R38" s="11">
+      <c r="R38" s="9">
         <v>1.1080000000000001</v>
       </c>
-      <c r="S38" s="13"/>
-      <c r="T38" s="13"/>
+      <c r="S38" s="11"/>
+      <c r="T38" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>